<commit_message>
Updated Richelieu SKU spec
</commit_message>
<xml_diff>
--- a/tests/ExcelLibrary.Tests/Unit/TestData/HafeleTest1.xlsx
+++ b/tests/ExcelLibrary.Tests/Unit/TestData/HafeleTest1.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nyop3\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zachary Londono\source\repos\RoyalExcelLibraryV2\tests\ExcelLibrary.Tests\Unit\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4480D3-A77C-45E5-9892-83E1329EC3A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="aJgl5B0saCaW7N7OJBzivcWbrgN47DPsZP7wUfrbm9Mr8SbjWwzM+9gaUaq5i9By/LBVhrKk15e0by/dv03wbg==" workbookSaltValue="hQzRumHje7A9HhMcA0I4Ng==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8565"/>
+    <workbookView xWindow="6645" yWindow="1005" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Order Sheet" sheetId="1" r:id="rId1"/>
@@ -90,17 +91,26 @@
     <definedName name="StateOptions">Data!$S$9:$S$21</definedName>
     <definedName name="StdMarkup">Data!$P$12</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Zachary Londono</author>
     <author>Drawer Department</author>
@@ -108,7 +118,7 @@
     <author>Hafele Drawer Department</author>
   </authors>
   <commentList>
-    <comment ref="J3" authorId="0" shapeId="0">
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -121,7 +131,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J4" authorId="0" shapeId="0">
+    <comment ref="J4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -134,7 +144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0">
+    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -147,7 +157,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J6" authorId="0" shapeId="0">
+    <comment ref="J6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -160,7 +170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J7" authorId="0" shapeId="0">
+    <comment ref="J7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -174,7 +184,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G9" authorId="1" shapeId="0">
+    <comment ref="G9" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -187,7 +197,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K10" authorId="1" shapeId="0">
+    <comment ref="K10" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -200,7 +210,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N10" authorId="0" shapeId="0">
+    <comment ref="N10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -214,7 +224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K11" authorId="1" shapeId="0">
+    <comment ref="K11" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -227,7 +237,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N11" authorId="1" shapeId="0">
+    <comment ref="N11" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -240,7 +250,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G13" authorId="2" shapeId="0">
+    <comment ref="G13" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -254,7 +264,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D14" authorId="3" shapeId="0">
+    <comment ref="D14" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -268,7 +278,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I15" authorId="0" shapeId="0">
+    <comment ref="I15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -281,7 +291,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L15" authorId="0" shapeId="0">
+    <comment ref="L15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -294,7 +304,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M15" authorId="0" shapeId="0">
+    <comment ref="M15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -307,7 +317,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O15" authorId="1" shapeId="0">
+    <comment ref="O15" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -320,7 +330,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S15" authorId="0" shapeId="0">
+    <comment ref="S15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -339,12 +349,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Zachary Londono</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -362,14 +372,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -384,7 +394,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="225">
   <si>
     <t>Height</t>
   </si>
@@ -1043,6 +1053,7 @@
         <sz val="10"/>
         <color theme="2" tint="-0.499984740745262"/>
         <rFont val="Aharoni"/>
+        <charset val="177"/>
       </rPr>
       <t>2.1.8</t>
     </r>
@@ -1080,11 +1091,14 @@
   <si>
     <t>alexcastrocw@gmail.com</t>
   </si>
+  <si>
+    <t>This is an order comment</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="10">
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -1097,7 +1111,7 @@
     <numFmt numFmtId="169" formatCode="000000\-00_);\(000000\-00\)"/>
     <numFmt numFmtId="170" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1232,6 +1246,7 @@
       <sz val="14"/>
       <color theme="2" tint="-0.499984740745262"/>
       <name val="Aharoni"/>
+      <charset val="177"/>
     </font>
     <font>
       <sz val="16"/>
@@ -1294,6 +1309,7 @@
       <sz val="10"/>
       <color theme="2" tint="-0.499984740745262"/>
       <name val="Aharoni"/>
+      <charset val="177"/>
     </font>
   </fonts>
   <fills count="14">
@@ -3128,7 +3144,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3F0060D1-2446-46EE-ACCA-F8D4B07EBB3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F0060D1-2446-46EE-ACCA-F8D4B07EBB3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3171,7 +3187,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CD6BDF1F-DCC7-402D-97D9-F1B7484709A4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD6BDF1F-DCC7-402D-97D9-F1B7484709A4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3220,7 +3236,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9186E791-A952-4D8B-A23D-7630F4F89E0D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9186E791-A952-4D8B-A23D-7630F4F89E0D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3545,7 +3561,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFD84C5D"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
@@ -3553,10 +3569,10 @@
   <dimension ref="A1:BD117"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="N11" sqref="N11:Q13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="67" customWidth="1"/>
     <col min="2" max="2" width="6.5703125" style="67" customWidth="1"/>
@@ -3609,12 +3625,12 @@
     <col min="58" max="16384" width="9.140625" style="67"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="19.5" customHeight="1" thickBot="1">
+    <row r="1" spans="1:56" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K1" s="69"/>
       <c r="N1" s="70"/>
       <c r="S1" s="136"/>
     </row>
-    <row r="2" spans="1:56" ht="23.25" customHeight="1">
+    <row r="2" spans="1:56" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="37"/>
       <c r="C2" s="88"/>
       <c r="D2" s="163"/>
@@ -3638,7 +3654,7 @@
       <c r="V2" s="216"/>
       <c r="W2" s="217"/>
     </row>
-    <row r="3" spans="1:56" ht="16.5" customHeight="1">
+    <row r="3" spans="1:56" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="41"/>
       <c r="C3" s="89"/>
       <c r="D3" s="164"/>
@@ -3668,7 +3684,7 @@
       </c>
       <c r="W3" s="208"/>
     </row>
-    <row r="4" spans="1:56" ht="16.5" customHeight="1">
+    <row r="4" spans="1:56" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="42"/>
       <c r="C4" s="90"/>
       <c r="D4" s="93"/>
@@ -3698,7 +3714,7 @@
       </c>
       <c r="W4" s="208"/>
     </row>
-    <row r="5" spans="1:56" ht="16.5" customHeight="1">
+    <row r="5" spans="1:56" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="42"/>
       <c r="C5" s="90"/>
       <c r="D5" s="93"/>
@@ -3731,7 +3747,7 @@
       </c>
       <c r="W5" s="208"/>
     </row>
-    <row r="6" spans="1:56" ht="16.5" customHeight="1">
+    <row r="6" spans="1:56" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="42"/>
       <c r="C6" s="90"/>
       <c r="D6" s="93"/>
@@ -3764,7 +3780,7 @@
       </c>
       <c r="W6" s="208"/>
     </row>
-    <row r="7" spans="1:56" ht="16.5" customHeight="1">
+    <row r="7" spans="1:56" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="42"/>
       <c r="C7" s="90"/>
       <c r="D7" s="93"/>
@@ -3796,7 +3812,7 @@
       </c>
       <c r="W7" s="208"/>
     </row>
-    <row r="8" spans="1:56" ht="16.5" customHeight="1" thickBot="1">
+    <row r="8" spans="1:56" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="42"/>
       <c r="C8" s="90"/>
       <c r="D8" s="93"/>
@@ -3845,7 +3861,7 @@
       <c r="AM8" s="25"/>
       <c r="AN8" s="25"/>
     </row>
-    <row r="9" spans="1:56" ht="16.5" customHeight="1" thickBot="1">
+    <row r="9" spans="1:56" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="43"/>
       <c r="C9" s="91"/>
       <c r="D9" s="165"/>
@@ -3881,7 +3897,7 @@
       <c r="AN9" s="25"/>
       <c r="AO9" s="25"/>
     </row>
-    <row r="10" spans="1:56" ht="16.5" customHeight="1" thickBot="1">
+    <row r="10" spans="1:56" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J10" s="48" t="s">
         <v>78</v>
       </c>
@@ -3919,7 +3935,7 @@
       <c r="AN10" s="25"/>
       <c r="AO10" s="25"/>
     </row>
-    <row r="11" spans="1:56" ht="16.5" customHeight="1" thickBot="1">
+    <row r="11" spans="1:56" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="30"/>
       <c r="C11" s="92"/>
       <c r="D11" s="92"/>
@@ -3937,7 +3953,9 @@
       <c r="K11" s="127">
         <v>709062730</v>
       </c>
-      <c r="N11" s="209"/>
+      <c r="N11" s="209" t="s">
+        <v>224</v>
+      </c>
       <c r="O11" s="210"/>
       <c r="P11" s="210"/>
       <c r="Q11" s="211"/>
@@ -3966,7 +3984,7 @@
       <c r="AN11" s="25"/>
       <c r="AO11" s="25"/>
     </row>
-    <row r="12" spans="1:56" ht="16.5" customHeight="1" thickBot="1">
+    <row r="12" spans="1:56" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="33"/>
       <c r="C12" s="93"/>
       <c r="D12" s="93"/>
@@ -4002,7 +4020,7 @@
       <c r="AN12" s="26"/>
       <c r="AO12" s="26"/>
     </row>
-    <row r="13" spans="1:56" ht="16.5" customHeight="1" thickBot="1">
+    <row r="13" spans="1:56" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="35"/>
       <c r="C13" s="94"/>
       <c r="D13" s="94"/>
@@ -4047,7 +4065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:56" ht="16.5" thickBot="1">
+    <row r="14" spans="1:56" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D14" s="198" t="s">
         <v>118</v>
       </c>
@@ -4109,7 +4127,7 @@
       </c>
       <c r="AS14" s="167"/>
     </row>
-    <row r="15" spans="1:56" s="74" customFormat="1" ht="21" customHeight="1" thickBot="1">
+    <row r="15" spans="1:56" s="74" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="53" t="s">
         <v>116</v>
       </c>
@@ -4279,7 +4297,7 @@
       </c>
       <c r="BD15" s="4"/>
     </row>
-    <row r="16" spans="1:56" ht="16.5">
+    <row r="16" spans="1:56" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="52">
         <f>ROW()-15</f>
         <v>1</v>
@@ -4466,7 +4484,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="17" spans="1:55" ht="16.5">
+    <row r="17" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <f t="shared" ref="A17:A80" si="21">ROW()-15</f>
         <v>2</v>
@@ -4653,7 +4671,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="18" spans="1:55" ht="16.5">
+    <row r="18" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <f t="shared" si="21"/>
         <v>3</v>
@@ -4852,7 +4870,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="19" spans="1:55" ht="16.5">
+    <row r="19" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
         <f t="shared" si="21"/>
         <v>4</v>
@@ -5042,7 +5060,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="20" spans="1:55" ht="16.5">
+    <row r="20" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
         <f t="shared" si="21"/>
         <v>5</v>
@@ -5231,7 +5249,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="21" spans="1:55" ht="16.5">
+    <row r="21" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
         <f t="shared" si="21"/>
         <v>6</v>
@@ -5420,7 +5438,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="22" spans="1:55" ht="16.5">
+    <row r="22" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A22" s="10">
         <f t="shared" si="21"/>
         <v>7</v>
@@ -5617,7 +5635,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="23" spans="1:55" ht="16.5">
+    <row r="23" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A23" s="10">
         <f t="shared" si="21"/>
         <v>8</v>
@@ -5806,7 +5824,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="24" spans="1:55" ht="16.5">
+    <row r="24" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A24" s="10">
         <f t="shared" si="21"/>
         <v>9</v>
@@ -5995,7 +6013,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="25" spans="1:55" ht="16.5">
+    <row r="25" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A25" s="10">
         <f t="shared" si="21"/>
         <v>10</v>
@@ -6184,7 +6202,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="26" spans="1:55" ht="16.5">
+    <row r="26" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A26" s="11">
         <f t="shared" si="21"/>
         <v>11</v>
@@ -6381,7 +6399,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="27" spans="1:55" ht="16.5">
+    <row r="27" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A27" s="11">
         <f t="shared" si="21"/>
         <v>12</v>
@@ -6570,7 +6588,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="28" spans="1:55" ht="16.5">
+    <row r="28" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A28" s="11">
         <f t="shared" si="21"/>
         <v>13</v>
@@ -6759,7 +6777,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="29" spans="1:55" ht="16.5">
+    <row r="29" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A29" s="11">
         <f t="shared" si="21"/>
         <v>14</v>
@@ -6948,7 +6966,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="30" spans="1:55" ht="16.5">
+    <row r="30" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A30" s="11">
         <f t="shared" si="21"/>
         <v>15</v>
@@ -7137,7 +7155,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="31" spans="1:55" ht="16.5">
+    <row r="31" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A31" s="11">
         <f t="shared" si="21"/>
         <v>16</v>
@@ -7326,7 +7344,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="32" spans="1:55" ht="16.5">
+    <row r="32" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A32" s="11">
         <f t="shared" si="21"/>
         <v>17</v>
@@ -7515,7 +7533,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="33" spans="1:55" ht="16.5">
+    <row r="33" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A33" s="11">
         <f t="shared" si="21"/>
         <v>18</v>
@@ -7704,7 +7722,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="34" spans="1:55" ht="16.5">
+    <row r="34" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A34" s="11">
         <f t="shared" si="21"/>
         <v>19</v>
@@ -7893,7 +7911,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="35" spans="1:55" ht="16.5">
+    <row r="35" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A35" s="11">
         <f t="shared" si="21"/>
         <v>20</v>
@@ -8082,7 +8100,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="36" spans="1:55" ht="16.5">
+    <row r="36" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A36" s="11">
         <f t="shared" si="21"/>
         <v>21</v>
@@ -8271,7 +8289,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="37" spans="1:55" ht="16.5">
+    <row r="37" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A37" s="11">
         <f t="shared" si="21"/>
         <v>22</v>
@@ -8460,7 +8478,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="38" spans="1:55" ht="16.5">
+    <row r="38" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A38" s="11">
         <f t="shared" si="21"/>
         <v>23</v>
@@ -8649,7 +8667,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="39" spans="1:55" ht="16.5">
+    <row r="39" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A39" s="11">
         <f t="shared" si="21"/>
         <v>24</v>
@@ -8838,7 +8856,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="40" spans="1:55" ht="16.5">
+    <row r="40" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A40" s="11">
         <f t="shared" si="21"/>
         <v>25</v>
@@ -9027,7 +9045,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="41" spans="1:55" ht="16.5">
+    <row r="41" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A41" s="11">
         <f t="shared" si="21"/>
         <v>26</v>
@@ -9216,7 +9234,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="42" spans="1:55" ht="16.5">
+    <row r="42" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A42" s="11">
         <f t="shared" si="21"/>
         <v>27</v>
@@ -9405,7 +9423,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="43" spans="1:55" ht="16.5">
+    <row r="43" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A43" s="11">
         <f t="shared" si="21"/>
         <v>28</v>
@@ -9594,7 +9612,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="44" spans="1:55" ht="16.5">
+    <row r="44" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A44" s="11">
         <f t="shared" si="21"/>
         <v>29</v>
@@ -9783,7 +9801,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="45" spans="1:55" ht="16.5">
+    <row r="45" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A45" s="11">
         <f t="shared" si="21"/>
         <v>30</v>
@@ -9972,7 +9990,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="46" spans="1:55" ht="16.5">
+    <row r="46" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A46" s="11">
         <f t="shared" si="21"/>
         <v>31</v>
@@ -10161,7 +10179,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="47" spans="1:55" ht="16.5">
+    <row r="47" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A47" s="11">
         <f t="shared" si="21"/>
         <v>32</v>
@@ -10350,7 +10368,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="48" spans="1:55" ht="16.5">
+    <row r="48" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A48" s="11">
         <f t="shared" si="21"/>
         <v>33</v>
@@ -10547,7 +10565,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="49" spans="1:55" ht="16.5">
+    <row r="49" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A49" s="11">
         <f t="shared" si="21"/>
         <v>34</v>
@@ -10736,7 +10754,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="50" spans="1:55" ht="16.5">
+    <row r="50" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A50" s="11">
         <f t="shared" si="21"/>
         <v>35</v>
@@ -10925,7 +10943,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="51" spans="1:55" ht="16.5">
+    <row r="51" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A51" s="11">
         <f t="shared" si="21"/>
         <v>36</v>
@@ -11114,7 +11132,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="52" spans="1:55" ht="16.5">
+    <row r="52" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A52" s="11">
         <f t="shared" si="21"/>
         <v>37</v>
@@ -11303,7 +11321,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="53" spans="1:55" ht="16.5">
+    <row r="53" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A53" s="11">
         <f t="shared" si="21"/>
         <v>38</v>
@@ -11492,7 +11510,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="54" spans="1:55" ht="16.5">
+    <row r="54" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A54" s="11">
         <f t="shared" si="21"/>
         <v>39</v>
@@ -11681,7 +11699,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="55" spans="1:55" ht="16.5">
+    <row r="55" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A55" s="11">
         <f t="shared" si="21"/>
         <v>40</v>
@@ -11870,7 +11888,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="56" spans="1:55" ht="16.5">
+    <row r="56" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A56" s="11">
         <f t="shared" si="21"/>
         <v>41</v>
@@ -12059,7 +12077,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="57" spans="1:55" ht="16.5">
+    <row r="57" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A57" s="11">
         <f t="shared" si="21"/>
         <v>42</v>
@@ -12248,7 +12266,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="58" spans="1:55" ht="16.5">
+    <row r="58" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A58" s="11">
         <f t="shared" si="21"/>
         <v>43</v>
@@ -12437,7 +12455,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="59" spans="1:55" ht="16.5">
+    <row r="59" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A59" s="11">
         <f t="shared" si="21"/>
         <v>44</v>
@@ -12626,7 +12644,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="60" spans="1:55" ht="16.5">
+    <row r="60" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A60" s="11">
         <f t="shared" si="21"/>
         <v>45</v>
@@ -12815,7 +12833,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="61" spans="1:55" ht="16.5">
+    <row r="61" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A61" s="11">
         <f t="shared" si="21"/>
         <v>46</v>
@@ -13004,7 +13022,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="62" spans="1:55" ht="16.5">
+    <row r="62" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A62" s="11">
         <f t="shared" si="21"/>
         <v>47</v>
@@ -13193,7 +13211,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="63" spans="1:55" ht="16.5">
+    <row r="63" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A63" s="11">
         <f t="shared" si="21"/>
         <v>48</v>
@@ -13382,7 +13400,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="64" spans="1:55" ht="16.5">
+    <row r="64" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A64" s="11">
         <f t="shared" si="21"/>
         <v>49</v>
@@ -13571,7 +13589,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="65" spans="1:55" ht="16.5">
+    <row r="65" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A65" s="11">
         <f t="shared" si="21"/>
         <v>50</v>
@@ -13760,7 +13778,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="66" spans="1:55" ht="16.5">
+    <row r="66" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A66" s="11">
         <f t="shared" si="21"/>
         <v>51</v>
@@ -13949,7 +13967,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="67" spans="1:55" ht="16.5">
+    <row r="67" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A67" s="11">
         <f t="shared" si="21"/>
         <v>52</v>
@@ -14138,7 +14156,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="68" spans="1:55" ht="16.5">
+    <row r="68" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A68" s="11">
         <f t="shared" si="21"/>
         <v>53</v>
@@ -14327,7 +14345,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="69" spans="1:55" ht="16.5">
+    <row r="69" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A69" s="11">
         <f t="shared" si="21"/>
         <v>54</v>
@@ -14516,7 +14534,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="70" spans="1:55" ht="16.5">
+    <row r="70" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A70" s="11">
         <f t="shared" si="21"/>
         <v>55</v>
@@ -14705,7 +14723,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="71" spans="1:55" ht="16.5">
+    <row r="71" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A71" s="11">
         <f t="shared" si="21"/>
         <v>56</v>
@@ -14894,7 +14912,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="72" spans="1:55" ht="16.5">
+    <row r="72" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A72" s="11">
         <f t="shared" si="21"/>
         <v>57</v>
@@ -15083,7 +15101,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="73" spans="1:55" ht="16.5">
+    <row r="73" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A73" s="11">
         <f t="shared" si="21"/>
         <v>58</v>
@@ -15272,7 +15290,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="74" spans="1:55" ht="16.5">
+    <row r="74" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A74" s="11">
         <f t="shared" si="21"/>
         <v>59</v>
@@ -15461,7 +15479,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="75" spans="1:55" ht="16.5">
+    <row r="75" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A75" s="11">
         <f t="shared" si="21"/>
         <v>60</v>
@@ -15650,7 +15668,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="76" spans="1:55" ht="16.5">
+    <row r="76" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A76" s="11">
         <f t="shared" si="21"/>
         <v>61</v>
@@ -15839,7 +15857,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="77" spans="1:55" ht="16.5">
+    <row r="77" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A77" s="11">
         <f t="shared" si="21"/>
         <v>62</v>
@@ -16028,7 +16046,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="78" spans="1:55" ht="16.5">
+    <row r="78" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A78" s="11">
         <f t="shared" si="21"/>
         <v>63</v>
@@ -16217,7 +16235,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="79" spans="1:55" ht="16.5">
+    <row r="79" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A79" s="11">
         <f t="shared" si="21"/>
         <v>64</v>
@@ -16406,7 +16424,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="80" spans="1:55" ht="16.5">
+    <row r="80" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A80" s="11">
         <f t="shared" si="21"/>
         <v>65</v>
@@ -16603,7 +16621,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="81" spans="1:55" ht="16.5">
+    <row r="81" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A81" s="11">
         <f t="shared" ref="A81:A116" si="82">ROW()-15</f>
         <v>66</v>
@@ -16792,7 +16810,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="82" spans="1:55" ht="16.5">
+    <row r="82" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A82" s="11">
         <f t="shared" si="82"/>
         <v>67</v>
@@ -16981,7 +16999,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="83" spans="1:55" ht="16.5">
+    <row r="83" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A83" s="11">
         <f t="shared" si="82"/>
         <v>68</v>
@@ -17170,7 +17188,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="84" spans="1:55" ht="16.5">
+    <row r="84" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A84" s="11">
         <f t="shared" si="82"/>
         <v>69</v>
@@ -17359,7 +17377,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="85" spans="1:55" ht="16.5">
+    <row r="85" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A85" s="11">
         <f t="shared" si="82"/>
         <v>70</v>
@@ -17548,7 +17566,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="86" spans="1:55" ht="16.5">
+    <row r="86" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A86" s="11">
         <f t="shared" si="82"/>
         <v>71</v>
@@ -17737,7 +17755,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="87" spans="1:55" ht="16.5">
+    <row r="87" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A87" s="11">
         <f t="shared" si="82"/>
         <v>72</v>
@@ -17926,7 +17944,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="88" spans="1:55" ht="16.5">
+    <row r="88" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A88" s="11">
         <f t="shared" si="82"/>
         <v>73</v>
@@ -18115,7 +18133,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="89" spans="1:55" ht="16.5">
+    <row r="89" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A89" s="11">
         <f t="shared" si="82"/>
         <v>74</v>
@@ -18304,7 +18322,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="90" spans="1:55" ht="16.5">
+    <row r="90" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A90" s="11">
         <f t="shared" si="82"/>
         <v>75</v>
@@ -18493,7 +18511,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="91" spans="1:55" ht="16.5">
+    <row r="91" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A91" s="11">
         <f t="shared" si="82"/>
         <v>76</v>
@@ -18682,7 +18700,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="92" spans="1:55" ht="16.5">
+    <row r="92" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A92" s="11">
         <f t="shared" si="82"/>
         <v>77</v>
@@ -18871,7 +18889,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="93" spans="1:55" ht="16.5">
+    <row r="93" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A93" s="11">
         <f t="shared" si="82"/>
         <v>78</v>
@@ -19060,7 +19078,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="94" spans="1:55" ht="16.5">
+    <row r="94" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A94" s="11">
         <f t="shared" si="82"/>
         <v>79</v>
@@ -19249,7 +19267,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="95" spans="1:55" ht="16.5">
+    <row r="95" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A95" s="11">
         <f t="shared" si="82"/>
         <v>80</v>
@@ -19438,7 +19456,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="96" spans="1:55" ht="16.5">
+    <row r="96" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A96" s="11">
         <f t="shared" si="82"/>
         <v>81</v>
@@ -19627,7 +19645,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="97" spans="1:55" ht="16.5">
+    <row r="97" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A97" s="11">
         <f t="shared" si="82"/>
         <v>82</v>
@@ -19816,7 +19834,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="98" spans="1:55" ht="16.5">
+    <row r="98" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A98" s="11">
         <f t="shared" si="82"/>
         <v>83</v>
@@ -20005,7 +20023,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="99" spans="1:55" ht="16.5">
+    <row r="99" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A99" s="11">
         <f t="shared" si="82"/>
         <v>84</v>
@@ -20194,7 +20212,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="100" spans="1:55" ht="16.5">
+    <row r="100" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A100" s="11">
         <f t="shared" si="82"/>
         <v>85</v>
@@ -20383,7 +20401,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="101" spans="1:55" ht="16.5">
+    <row r="101" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A101" s="11">
         <f t="shared" si="82"/>
         <v>86</v>
@@ -20572,7 +20590,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="102" spans="1:55" ht="16.5">
+    <row r="102" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A102" s="11">
         <f t="shared" si="82"/>
         <v>87</v>
@@ -20761,7 +20779,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="103" spans="1:55" ht="16.5">
+    <row r="103" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A103" s="11">
         <f t="shared" si="82"/>
         <v>88</v>
@@ -20950,7 +20968,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="104" spans="1:55" ht="16.5">
+    <row r="104" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A104" s="11">
         <f t="shared" si="82"/>
         <v>89</v>
@@ -21139,7 +21157,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="105" spans="1:55" ht="16.5">
+    <row r="105" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A105" s="11">
         <f t="shared" si="82"/>
         <v>90</v>
@@ -21328,7 +21346,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="106" spans="1:55" ht="16.5">
+    <row r="106" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A106" s="11">
         <f t="shared" si="82"/>
         <v>91</v>
@@ -21517,7 +21535,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="107" spans="1:55" ht="16.5">
+    <row r="107" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A107" s="11">
         <f t="shared" si="82"/>
         <v>92</v>
@@ -21706,7 +21724,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="108" spans="1:55" ht="16.5">
+    <row r="108" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A108" s="11">
         <f t="shared" si="82"/>
         <v>93</v>
@@ -21895,7 +21913,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="109" spans="1:55" ht="16.5">
+    <row r="109" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A109" s="11">
         <f t="shared" si="82"/>
         <v>94</v>
@@ -22084,7 +22102,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="110" spans="1:55" ht="16.5">
+    <row r="110" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A110" s="11">
         <f t="shared" si="82"/>
         <v>95</v>
@@ -22273,7 +22291,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="111" spans="1:55" ht="16.5">
+    <row r="111" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A111" s="11">
         <f t="shared" si="82"/>
         <v>96</v>
@@ -22462,7 +22480,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="112" spans="1:55" ht="16.5">
+    <row r="112" spans="1:55" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A112" s="11">
         <f t="shared" si="82"/>
         <v>97</v>
@@ -22651,7 +22669,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="113" spans="1:56" ht="16.5">
+    <row r="113" spans="1:56" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A113" s="11">
         <f t="shared" si="82"/>
         <v>98</v>
@@ -22840,7 +22858,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="114" spans="1:56" ht="16.5">
+    <row r="114" spans="1:56" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A114" s="11">
         <f t="shared" si="82"/>
         <v>99</v>
@@ -23029,7 +23047,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="115" spans="1:56" ht="16.5">
+    <row r="115" spans="1:56" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A115" s="11">
         <f t="shared" si="82"/>
         <v>100</v>
@@ -23218,7 +23236,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="116" spans="1:56" ht="16.5">
+    <row r="116" spans="1:56" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A116" s="11">
         <f t="shared" si="82"/>
         <v>101</v>
@@ -23407,7 +23425,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="117" spans="1:56">
+    <row r="117" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A117" s="15" t="s">
         <v>16</v>
       </c>
@@ -23579,7 +23597,7 @@
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="gpgvlQ18hYxvrn3mH2IH6r06u3MPcs1wxuh4ngV0HkaBgO8pSnXnWBiAEHoWrBfW6/3A6gn6ftUyTpM9rchehA==" saltValue="2L5PD1ioMtxdnE5l5COW/A==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" deleteRows="0" sort="0"/>
-  <sortState ref="B16:L47">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B16:L47">
     <sortCondition ref="D16:D47"/>
   </sortState>
   <mergeCells count="26">
@@ -23929,91 +23947,91 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="27">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must select only from the pull-down list." sqref="G3:H3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must select only from the pull-down list." sqref="G3:H3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Materials</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7:H7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7:H7" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>ClipOptions</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K13" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Fraction,Decimal,Metric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enter &quot;Yes&quot; only to trigger logos globally." sqref="G6:H6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enter &quot;Yes&quot; only to trigger logos globally." sqref="G6:H6" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"Yes,Yes - With Setup,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="You can only enter &quot;Yes&quot; or &quot;No&quot;" sqref="G8:H9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="You can only enter &quot;Yes&quot; or &quot;No&quot;" sqref="G8:H9" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must select only from the pull-down list." sqref="G4:H4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must select only from the pull-down list." sqref="G4:H4" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>Bottoms</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must select only from the pull-down list." sqref="G5:H5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must select only from the pull-down list." sqref="G5:H5" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>Notches</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K8:M8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K8:M8" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>ProductionTime</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" error="Invalid Accessory Option" sqref="N16:N116">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" error="Invalid Accessory Option" sqref="N16:N116" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>Accessories</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid Clip Option" sqref="M16:M116">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid Clip Option" sqref="M16:M116" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>ClipOptions</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid Notch Option." sqref="K16:K116">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid Notch Option." sqref="K16:K116" xr:uid="{00000000-0002-0000-0000-00000A000000}">
       <formula1>Notches</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid Bottom Material. Please enter valid bottom material for accurate pricing." sqref="J16:J116">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Invalid Bottom Material. Please enter valid bottom material for accurate pricing." sqref="J16:J116" xr:uid="{00000000-0002-0000-0000-00000B000000}">
       <formula1>Bottoms</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Non-Standard heights are more expensive than standard heights." sqref="F16:F116">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Non-Standard heights are more expensive than standard heights." sqref="F16:F116" xr:uid="{00000000-0002-0000-0000-00000C000000}">
       <formula1>IF(Notation="Metric", MetricHeights,Heights)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="You can only enter &quot;Scoop Front&quot; here for a roll-out type drawer." sqref="I16:I116">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="You can only enter &quot;Scoop Front&quot; here for a roll-out type drawer." sqref="I16:I116" xr:uid="{00000000-0002-0000-0000-00000D000000}">
       <formula1>"Scoop Front"</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enter a whole number only and warning given for over 99 of one item?" sqref="B16:B116">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enter a whole number only and warning given for over 99 of one item?" sqref="B16:B116" xr:uid="{00000000-0002-0000-0000-00000E000000}">
       <formula1>1</formula1>
       <formula2>99</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" error="Invalid Logo Option" sqref="L16:L116">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" error="Invalid Logo Option" sqref="L16:L116" xr:uid="{00000000-0002-0000-0000-00000F000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14" xr:uid="{00000000-0002-0000-0000-000010000000}">
       <formula1>OpeningSizes</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Maximum height of 99&quot;" sqref="D16:D116">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Maximum height of 99&quot;" sqref="D16:D116" xr:uid="{00000000-0002-0000-0000-000011000000}">
       <formula1>1</formula1>
       <formula2>99*IF(Notation="Metric",25.4,1)</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" error="Minimum width is 6&quot; and maximum width is 52&quot;." sqref="G117">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" error="Minimum width is 6&quot; and maximum width is 52&quot;." sqref="G117" xr:uid="{00000000-0002-0000-0000-000012000000}">
       <formula1>IF(Notation="Metric",6*25.4,6)</formula1>
       <formula2>IF(Notation="Metric",52*25.4,52)</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Minimum width is 6&quot; and maximum width is 52&quot;." sqref="G16:G116">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Minimum width is 6&quot; and maximum width is 52&quot;." sqref="G16:G116" xr:uid="{00000000-0002-0000-0000-000013000000}">
       <formula1>IF(Notation="Metric",6*25.4,6)</formula1>
       <formula2>IF(Notation="Metric",52*25.4,52)</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Minimum drawer box depth is 5&quot; and maximum depth is 36&quot;." sqref="H16:H116">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Minimum drawer box depth is 5&quot; and maximum depth is 36&quot;." sqref="H16:H116" xr:uid="{00000000-0002-0000-0000-000014000000}">
       <formula1>5*IF(Notation="Metric",25.4,1)</formula1>
       <formula2>36*IF(Notation="Metric",25.4,1)</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U16:W116">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U16:W116" xr:uid="{00000000-0002-0000-0000-000015000000}">
       <formula1>0</formula1>
       <formula2>999</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Maximum width of 99&quot;" sqref="E16:E116">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Maximum width of 99&quot;" sqref="E16:E116" xr:uid="{00000000-0002-0000-0000-000016000000}">
       <formula1>1</formula1>
       <formula2>99*IF(Notation="Metric",25.4,1)</formula2>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enter a whole number only and warning given for over 99 of one item?" sqref="C16:C116"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Use 2 character state abbreviation" sqref="V8:W8"/>
-    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Order Date" error="You must enter a valid date, no earlier then today" sqref="K3:L3"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V4:W4">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enter a whole number only and warning given for over 99 of one item?" sqref="C16:C116" xr:uid="{00000000-0002-0000-0000-000017000000}"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Use 2 character state abbreviation" sqref="V8:W8" xr:uid="{00000000-0002-0000-0000-000018000000}"/>
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Order Date" error="You must enter a valid date, no earlier then today" sqref="K3:L3" xr:uid="{00000000-0002-0000-0000-000019000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V4:W4" xr:uid="{00000000-0002-0000-0000-00001A000000}">
       <formula1>OFFSET(CompanyNames,0,0, COUNTIF(CompanyNames, "&lt;&gt;"), 1)</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="O8" r:id="rId1"/>
+    <hyperlink ref="O8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.27" right="0.18" top="0.54" bottom="0.37" header="0.3" footer="0.18"/>
   <pageSetup scale="80" fitToHeight="0" orientation="landscape" r:id="rId2"/>
@@ -24030,7 +24048,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet5">
     <tabColor rgb="FF7030A0"/>
     <pageSetUpPr fitToPage="1"/>
@@ -24041,7 +24059,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
@@ -24052,7 +24070,7 @@
     <col min="9" max="9" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="146" customFormat="1" ht="16.5" thickBot="1">
+    <row r="1" spans="1:9" s="146" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="174" t="s">
         <v>13</v>
       </c>
@@ -24081,10 +24099,10 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I2" s="181"/>
     </row>
-    <row r="203" spans="1:9">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" s="180" t="s">
         <v>195</v>
       </c>
@@ -24124,7 +24142,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2">
     <tabColor theme="7" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
@@ -24133,7 +24151,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="15.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" style="1" customWidth="1"/>
@@ -24141,7 +24159,7 @@
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.25" customHeight="1">
+    <row r="1" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="121"/>
       <c r="B1" s="122"/>
       <c r="C1" s="122" t="s">
@@ -24159,7 +24177,7 @@
         <v>7998</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="124" t="s">
         <v>63</v>
       </c>
@@ -24182,14 +24200,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="E4" s="14"/>
@@ -24199,7 +24217,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="E5" s="14"/>
@@ -24209,7 +24227,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="E6" s="14"/>
@@ -24219,7 +24237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="D7" s="14"/>
@@ -24230,7 +24248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="D8" s="14"/>
@@ -24241,7 +24259,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
       <c r="D9" s="14"/>
@@ -24252,7 +24270,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="14"/>
       <c r="D10" s="14"/>
@@ -24263,7 +24281,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="14"/>
       <c r="D11" s="14"/>
@@ -24274,7 +24292,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -24283,7 +24301,7 @@
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -24292,7 +24310,7 @@
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -24301,7 +24319,7 @@
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
@@ -24322,7 +24340,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:G2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:G2" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>CutPasteOptions</formula1>
     </dataValidation>
   </dataValidations>
@@ -24337,7 +24355,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4">
     <tabColor theme="4" tint="0.59999389629810485"/>
     <pageSetUpPr fitToPage="1"/>
@@ -24348,7 +24366,7 @@
       <selection activeCell="E1" sqref="E1:R1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" customWidth="1"/>
@@ -24360,7 +24378,7 @@
     <col min="29" max="29" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="148" t="s">
         <v>134</v>
       </c>
@@ -24382,7 +24400,7 @@
       <c r="Q1" s="168"/>
       <c r="R1" s="168"/>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="148" t="s">
         <v>174</v>
       </c>
@@ -24414,7 +24432,7 @@
       <c r="AB2" s="225"/>
       <c r="AC2" s="225"/>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="149"/>
       <c r="B3" s="150"/>
       <c r="C3" s="150"/>
@@ -24456,7 +24474,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="225" t="s">
         <v>184</v>
       </c>
@@ -24490,7 +24508,7 @@
       <c r="AB4" s="148"/>
       <c r="AC4" s="148"/>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="148" t="s">
         <v>177</v>
       </c>
@@ -24509,7 +24527,7 @@
       <c r="AB5" s="148"/>
       <c r="AC5" s="148"/>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="str">
         <f>IF(ClipSelection="","",VLOOKUP(ClipSelection,ClipMatrix,2,FALSE))</f>
         <v/>
@@ -24530,7 +24548,7 @@
       <c r="AB6" s="148"/>
       <c r="AC6" s="148"/>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="str">
         <f>IF(ClipSelection="","",IF(VLOOKUP(ClipSelection,ClipMatrix,3,FALSE)&lt;&gt;"",VLOOKUP(ClipSelection,ClipMatrix,3,FALSE),""))</f>
         <v/>
@@ -24557,7 +24575,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="158"/>
       <c r="B8" s="158"/>
       <c r="W8" s="184">
@@ -24572,7 +24590,7 @@
       <c r="AB8" s="148"/>
       <c r="AC8" s="148"/>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="225" t="s">
         <v>183</v>
       </c>
@@ -24608,7 +24626,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="148" t="s">
         <v>135</v>
       </c>
@@ -24679,7 +24697,7 @@
       <c r="AB10" s="148"/>
       <c r="AC10" s="148"/>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="162">
         <f t="array" ref="A11">IFERROR(INDEX('Order Sheet'!$H$16:$H$116,MATCH(0,COUNTIF(A$10:A10,'Order Sheet'!$H$16:$H$116),0)), "")</f>
         <v>12</v>
@@ -24772,7 +24790,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="162" t="str">
         <f t="array" aca="1" ref="A12" ca="1">IFERROR(INDEX('Order Sheet'!$H$16:$H$116,MATCH(0,COUNTIF(A$10:A11,'Order Sheet'!$H$16:$H$116),0)), "")</f>
         <v/>
@@ -24858,7 +24876,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="162" t="str">
         <f t="array" aca="1" ref="A13" ca="1">IFERROR(INDEX('Order Sheet'!$H$16:$H$116,MATCH(0,COUNTIF(A$10:A12,'Order Sheet'!$H$16:$H$116),0)), "")</f>
         <v/>
@@ -24950,7 +24968,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="162" t="str">
         <f t="array" aca="1" ref="A14" ca="1">IFERROR(INDEX('Order Sheet'!$H$16:$H$116,MATCH(0,COUNTIF(A$10:A13,'Order Sheet'!$H$16:$H$116),0)), "")</f>
         <v/>
@@ -25036,7 +25054,7 @@
       <c r="AB14" s="148"/>
       <c r="AC14" s="148"/>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="162" t="str">
         <f t="array" aca="1" ref="A15" ca="1">IFERROR(INDEX('Order Sheet'!$H$16:$H$116,MATCH(0,COUNTIF(A$10:A14,'Order Sheet'!$H$16:$H$116),0)), "")</f>
         <v/>
@@ -25122,7 +25140,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="162" t="str">
         <f t="array" aca="1" ref="A16" ca="1">IFERROR(INDEX('Order Sheet'!$H$16:$H$116,MATCH(0,COUNTIF(A$10:A15,'Order Sheet'!$H$16:$H$116),0)), "")</f>
         <v/>
@@ -25213,7 +25231,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="17" spans="1:29">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="162" t="str">
         <f t="array" aca="1" ref="A17" ca="1">IFERROR(INDEX('Order Sheet'!$H$16:$H$116,MATCH(0,COUNTIF(A$10:A16,'Order Sheet'!$H$16:$H$116),0)), "")</f>
         <v/>
@@ -25298,7 +25316,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="18" spans="1:29">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="162" t="str">
         <f t="array" aca="1" ref="A18" ca="1">IFERROR(INDEX('Order Sheet'!$H$16:$H$116,MATCH(0,COUNTIF(A$10:A17,'Order Sheet'!$H$16:$H$116),0)), "")</f>
         <v/>
@@ -25372,7 +25390,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="1:29">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="162" t="str">
         <f t="array" aca="1" ref="A19" ca="1">IFERROR(INDEX('Order Sheet'!$H$16:$H$116,MATCH(0,COUNTIF(A$10:A18,'Order Sheet'!$H$16:$H$116),0)), "")</f>
         <v/>
@@ -25451,7 +25469,7 @@
       <c r="X19" s="190"/>
       <c r="Y19" s="190"/>
     </row>
-    <row r="20" spans="1:29">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="162" t="str">
         <f t="array" aca="1" ref="A20" ca="1">IFERROR(INDEX('Order Sheet'!$H$16:$H$116,MATCH(0,COUNTIF(A$10:A19,'Order Sheet'!$H$16:$H$116),0)), "")</f>
         <v/>
@@ -25534,7 +25552,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="21" spans="1:29">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="162" t="str">
         <f t="array" aca="1" ref="A21" ca="1">IFERROR(INDEX('Order Sheet'!$H$16:$H$116,MATCH(0,COUNTIF(A$10:A20,'Order Sheet'!$H$16:$H$116),0)), "")</f>
         <v/>
@@ -25615,7 +25633,7 @@
       </c>
       <c r="Y21" s="190"/>
     </row>
-    <row r="22" spans="1:29">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="162" t="str">
         <f t="array" aca="1" ref="A22" ca="1">IFERROR(INDEX('Order Sheet'!$H$16:$H$116,MATCH(0,COUNTIF(A$10:A21,'Order Sheet'!$H$16:$H$116),0)), "")</f>
         <v/>
@@ -25696,7 +25714,7 @@
       </c>
       <c r="Y22" s="190"/>
     </row>
-    <row r="23" spans="1:29">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="162" t="str">
         <f t="array" aca="1" ref="A23" ca="1">IFERROR(INDEX('Order Sheet'!$H$16:$H$116,MATCH(0,COUNTIF(A$10:A22,'Order Sheet'!$H$16:$H$116),0)), "")</f>
         <v/>
@@ -25777,7 +25795,7 @@
       </c>
       <c r="Y23" s="190"/>
     </row>
-    <row r="24" spans="1:29">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="162" t="str">
         <f t="array" aca="1" ref="A24" ca="1">IFERROR(INDEX('Order Sheet'!$H$16:$H$116,MATCH(0,COUNTIF(A$10:A23,'Order Sheet'!$H$16:$H$116),0)), "")</f>
         <v/>
@@ -25858,7 +25876,7 @@
       </c>
       <c r="Y24" s="190"/>
     </row>
-    <row r="25" spans="1:29">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="162" t="str">
         <f t="array" aca="1" ref="A25" ca="1">IFERROR(INDEX('Order Sheet'!$H$16:$H$116,MATCH(0,COUNTIF(A$10:A24,'Order Sheet'!$H$16:$H$116),0)), "")</f>
         <v/>
@@ -25939,7 +25957,7 @@
       </c>
       <c r="Y25" s="190"/>
     </row>
-    <row r="26" spans="1:29">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="162" t="str">
         <f t="array" aca="1" ref="A26" ca="1">IFERROR(INDEX('Order Sheet'!$H$16:$H$116,MATCH(0,COUNTIF(A$10:A25,'Order Sheet'!$H$16:$H$116),0)), "")</f>
         <v/>
@@ -26020,7 +26038,7 @@
       </c>
       <c r="Y26" s="190"/>
     </row>
-    <row r="27" spans="1:29">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="162" t="str">
         <f t="array" aca="1" ref="A27" ca="1">IFERROR(INDEX('Order Sheet'!$H$16:$H$116,MATCH(0,COUNTIF(A$10:A26,'Order Sheet'!$H$16:$H$116),0)), "")</f>
         <v/>
@@ -26103,7 +26121,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="28" spans="1:29">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="162" t="str">
         <f t="array" aca="1" ref="A28" ca="1">IFERROR(INDEX('Order Sheet'!$H$16:$H$116,MATCH(0,COUNTIF(A$10:A27,'Order Sheet'!$H$16:$H$116),0)), "")</f>
         <v/>
@@ -26184,7 +26202,7 @@
       </c>
       <c r="Y28" s="190"/>
     </row>
-    <row r="29" spans="1:29">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="162" t="str">
         <f t="array" aca="1" ref="A29" ca="1">IFERROR(INDEX('Order Sheet'!$H$16:$H$116,MATCH(0,COUNTIF(A$10:A28,'Order Sheet'!$H$16:$H$116),0)), "")</f>
         <v/>
@@ -26267,7 +26285,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="30" spans="1:29">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="162" t="str">
         <f t="array" aca="1" ref="A30" ca="1">IFERROR(INDEX('Order Sheet'!$H$16:$H$116,MATCH(0,COUNTIF(A$10:A29,'Order Sheet'!$H$16:$H$116),0)), "")</f>
         <v/>
@@ -26341,7 +26359,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="31" spans="1:29">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="162" t="str">
         <f t="array" aca="1" ref="A31" ca="1">IFERROR(INDEX('Order Sheet'!$H$16:$H$116,MATCH(0,COUNTIF(A$10:A30,'Order Sheet'!$H$16:$H$116),0)), "")</f>
         <v/>
@@ -26418,7 +26436,7 @@
       <c r="X31" s="155"/>
       <c r="Y31" s="156"/>
     </row>
-    <row r="32" spans="1:29">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" s="157" t="s">
         <v>16</v>
       </c>
@@ -26449,17 +26467,17 @@
       <c r="X32" s="155"/>
       <c r="Y32" s="156"/>
     </row>
-    <row r="34" spans="23:25">
+    <row r="34" spans="23:25" x14ac:dyDescent="0.25">
       <c r="W34" s="153"/>
       <c r="X34" s="154"/>
       <c r="Y34" s="154"/>
     </row>
-    <row r="35" spans="23:25">
+    <row r="35" spans="23:25" x14ac:dyDescent="0.25">
       <c r="W35" s="153"/>
       <c r="X35" s="154"/>
       <c r="Y35" s="154"/>
     </row>
-    <row r="36" spans="23:25">
+    <row r="36" spans="23:25" x14ac:dyDescent="0.25">
       <c r="W36" s="153"/>
       <c r="X36" s="154"/>
       <c r="Y36" s="154"/>
@@ -26484,13 +26502,13 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="C11:C31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="C11:C31" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>SlideBrands</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:R2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:R2" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>ClipNames</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:R1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:R1" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>SlideBrands</formula1>
     </dataValidation>
   </dataValidations>
@@ -26504,7 +26522,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:Z25"/>
   <sheetViews>
@@ -26512,7 +26530,7 @@
       <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="67" customWidth="1"/>
     <col min="2" max="2" width="15" style="67" bestFit="1" customWidth="1"/>
@@ -26538,7 +26556,7 @@
     <col min="22" max="16384" width="9.140625" style="67"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26">
+    <row r="1" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B1" s="78" t="s">
         <v>188</v>
       </c>
@@ -26546,7 +26564,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:26">
+    <row r="2" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B2" s="78" t="s">
         <v>21</v>
       </c>
@@ -26601,7 +26619,7 @@
       <c r="Y2" s="226"/>
       <c r="Z2" s="226"/>
     </row>
-    <row r="3" spans="2:26">
+    <row r="3" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B3" s="173">
         <v>2.5</v>
       </c>
@@ -26660,7 +26678,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="2:26">
+    <row r="4" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B4" s="173">
         <v>3.375</v>
       </c>
@@ -26722,7 +26740,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:26">
+    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B5" s="173">
         <v>4.125</v>
       </c>
@@ -26783,7 +26801,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="2:26">
+    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B6" s="173">
         <v>5.375</v>
       </c>
@@ -26844,7 +26862,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="2:26">
+    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B7" s="173">
         <v>6.25</v>
       </c>
@@ -26877,7 +26895,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="8" spans="2:26">
+    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B8" s="173">
         <v>7.125</v>
       </c>
@@ -26922,7 +26940,7 @@
         <v>11.08</v>
       </c>
     </row>
-    <row r="9" spans="2:26">
+    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B9" s="173">
         <v>8.25</v>
       </c>
@@ -26961,7 +26979,7 @@
         <v>14.77</v>
       </c>
     </row>
-    <row r="10" spans="2:26">
+    <row r="10" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B10" s="173">
         <v>9.25</v>
       </c>
@@ -27006,7 +27024,7 @@
         <v>18.46</v>
       </c>
     </row>
-    <row r="11" spans="2:26">
+    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B11" s="173">
         <v>10.25</v>
       </c>
@@ -27045,7 +27063,7 @@
         <v>23.08</v>
       </c>
     </row>
-    <row r="12" spans="2:26">
+    <row r="12" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B12" s="173">
         <v>12</v>
       </c>
@@ -27090,7 +27108,7 @@
         <v>26.77</v>
       </c>
     </row>
-    <row r="13" spans="2:26">
+    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
       <c r="I13" s="81" t="s">
         <v>32</v>
       </c>
@@ -27110,7 +27128,7 @@
         <v>32.31</v>
       </c>
     </row>
-    <row r="14" spans="2:26">
+    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B14" s="86"/>
       <c r="C14" s="86"/>
       <c r="D14" s="86"/>
@@ -27142,7 +27160,7 @@
         <v>36.92</v>
       </c>
     </row>
-    <row r="15" spans="2:26">
+    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B15" s="86"/>
       <c r="C15" s="86"/>
       <c r="D15" s="86"/>
@@ -27168,7 +27186,7 @@
         <v>43.38</v>
       </c>
     </row>
-    <row r="16" spans="2:26">
+    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B16" s="86"/>
       <c r="C16" s="86"/>
       <c r="D16" s="86"/>
@@ -27197,7 +27215,7 @@
         <v>2.31</v>
       </c>
     </row>
-    <row r="17" spans="2:22">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B17" s="86"/>
       <c r="C17" s="86"/>
       <c r="D17" s="86"/>
@@ -27223,7 +27241,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:22">
+    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B18" s="86"/>
       <c r="C18" s="86"/>
       <c r="D18" s="86"/>
@@ -27250,7 +27268,7 @@
         <v>1.5384615384615383</v>
       </c>
     </row>
-    <row r="19" spans="2:22">
+    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B19" s="86"/>
       <c r="C19" s="86"/>
       <c r="D19" s="86"/>
@@ -27271,7 +27289,7 @@
         <v>2.3076923076923075</v>
       </c>
     </row>
-    <row r="20" spans="2:22">
+    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B20" s="86"/>
       <c r="C20" s="86"/>
       <c r="D20" s="86"/>
@@ -27292,7 +27310,7 @@
         <v>5.3846153846153841</v>
       </c>
     </row>
-    <row r="21" spans="2:22">
+    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B21" s="86"/>
       <c r="C21" s="86"/>
       <c r="D21" s="86"/>
@@ -27309,7 +27327,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="2:22">
+    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B22" s="86"/>
       <c r="C22" s="86"/>
       <c r="D22" s="86"/>
@@ -27319,12 +27337,12 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="2:22">
+    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
       <c r="L23" s="81">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="2:22">
+    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
       <c r="U24" s="141" t="s">
         <v>88</v>
       </c>
@@ -27332,7 +27350,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="2:22">
+    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
       <c r="U25" s="141" t="s">
         <v>89</v>
       </c>
@@ -27342,7 +27360,7 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" insertColumns="0" insertRows="0"/>
-  <sortState ref="S9:S21">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="S9:S21">
     <sortCondition ref="S9:S21"/>
   </sortState>
   <mergeCells count="2">

</xml_diff>